<commit_message>
Alu debug Test 1 Passed
PcRegRwTest passed
</commit_message>
<xml_diff>
--- a/Docs/AHPL/Decodificador ALU.xlsx
+++ b/Docs/AHPL/Decodificador ALU.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejaverianaedu.sharepoint.com/sites/TrabajodegradoprocesadorRISC-V/Shared Documents/General/Documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{7FB4B74B-5C74-4AFF-8E3E-9FF489F3BC51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B342E016-C186-4951-A0E6-1ADBDBB436F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EAAF5E-2281-4A87-B383-A77CED115C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4245" yWindow="975" windowWidth="21600" windowHeight="11385" xr2:uid="{BDB51A68-6DFE-41A4-B120-9DBE7CEC98C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BDB51A68-6DFE-41A4-B120-9DBE7CEC98C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,9 +40,9 @@
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{57C3056A-A932-44E4-BB79-DFEA048C4124}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t xml:space="preserve">[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     Los datos del IR corresponden a la señal de IR_ALU - 7 ej, IR(12)= IR_ALU(5)
 </t>
       </text>
@@ -214,7 +214,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,7 +284,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -592,22 +592,22 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="H9" sqref="A8:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="33.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45">
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -659,7 +659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -685,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -711,7 +711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -737,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -763,7 +763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -789,7 +789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -815,7 +815,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -841,7 +841,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -867,7 +867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -893,7 +893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -919,7 +919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -945,7 +945,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -971,7 +971,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -997,7 +997,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -1613,6 +1613,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100499B73C812517E4B87BCDE641853BAB9" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b68fceede8c5805f76295220e8e44f13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad4fc1d6-332d-474d-af02-ccba7dd3642b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585d2332b120932ddf2a11d4d4e88441" ns2:_="">
     <xsd:import namespace="ad4fc1d6-332d-474d-af02-ccba7dd3642b"/>
@@ -1784,20 +1790,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E65CB590-09DC-46F2-A9AB-B5C44E755103}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E65CB590-09DC-46F2-A9AB-B5C44E755103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F147EB6E-6B34-41BD-9106-733B66C83C05}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{041AE642-E628-4978-88CE-A3DA4D4C3956}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{041AE642-E628-4978-88CE-A3DA4D4C3956}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F147EB6E-6B34-41BD-9106-733B66C83C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ad4fc1d6-332d-474d-af02-ccba7dd3642b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
shift bugfix irq2 sim complete
</commit_message>
<xml_diff>
--- a/Docs/AHPL/Decodificador ALU.xlsx
+++ b/Docs/AHPL/Decodificador ALU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EAAF5E-2281-4A87-B383-A77CED115C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEC765A-6E79-4F82-AFBF-72479D91493C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BDB51A68-6DFE-41A4-B120-9DBE7CEC98C2}"/>
   </bookViews>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789F5470-5CE4-4FE5-A5AA-D34553BCB0AA}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="A8:H9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,7 +603,7 @@
     <col min="4" max="4" width="21.5546875" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="47.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1613,12 +1613,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100499B73C812517E4B87BCDE641853BAB9" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b68fceede8c5805f76295220e8e44f13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad4fc1d6-332d-474d-af02-ccba7dd3642b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585d2332b120932ddf2a11d4d4e88441" ns2:_="">
     <xsd:import namespace="ad4fc1d6-332d-474d-af02-ccba7dd3642b"/>
@@ -1790,6 +1784,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E65CB590-09DC-46F2-A9AB-B5C44E755103}">
   <ds:schemaRefs>
@@ -1799,15 +1799,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{041AE642-E628-4978-88CE-A3DA4D4C3956}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F147EB6E-6B34-41BD-9106-733B66C83C05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1823,4 +1814,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{041AE642-E628-4978-88CE-A3DA4D4C3956}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>